<commit_message>
user admin role 부여 취약점 수정
</commit_message>
<xml_diff>
--- a/secure-coding-checklist.xlsx
+++ b/secure-coding-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\barrack\white_hat_school\secure_coding\secure-coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA019FC-0D96-41FF-B5AC-2C87A70D1615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD5820B-1D68-4631-A7E7-56404145DB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15540" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="기능구현 함수" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="78">
   <si>
     <t>입력데이터검증및표현</t>
   </si>
@@ -641,8 +641,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -888,8 +888,8 @@
   </sheetPr>
   <dimension ref="B2:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -942,7 +942,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.45">
@@ -1006,7 +1009,10 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.45">
@@ -1017,7 +1023,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>26</v>
       </c>
@@ -1025,28 +1031,34 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +1066,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>12</v>
       </c>
@@ -1062,7 +1074,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
         <v>13</v>
       </c>
@@ -1070,20 +1082,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
         <v>27</v>
       </c>
@@ -1091,7 +1106,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
         <v>28</v>
       </c>
@@ -1099,12 +1114,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C29" t="s">
         <v>17</v>
       </c>
@@ -1112,7 +1127,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
         <v>18</v>
       </c>
@@ -1120,12 +1135,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C32" t="s">
         <v>20</v>
       </c>
@@ -1133,7 +1148,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C33" t="s">
         <v>21</v>
       </c>
@@ -1141,7 +1156,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C34" t="s">
         <v>22</v>
       </c>
@@ -1149,12 +1164,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C36" t="s">
         <v>37</v>
       </c>
@@ -1162,14 +1177,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C37" t="s">
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1186,8 +1198,8 @@
   </sheetPr>
   <dimension ref="B2:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1240,7 +1252,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.45">
@@ -1304,7 +1319,10 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.45">
@@ -1315,7 +1333,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>26</v>
       </c>
@@ -1323,20 +1341,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>10</v>
       </c>
@@ -1344,7 +1365,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
         <v>11</v>
       </c>
@@ -1352,7 +1373,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>12</v>
       </c>
@@ -1360,28 +1381,34 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
         <v>27</v>
       </c>
@@ -1389,7 +1416,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
         <v>28</v>
       </c>
@@ -1397,12 +1424,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C29" t="s">
         <v>17</v>
       </c>
@@ -1410,7 +1437,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
         <v>18</v>
       </c>
@@ -1418,12 +1445,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C32" t="s">
         <v>20</v>
       </c>
@@ -1431,7 +1458,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C33" t="s">
         <v>21</v>
       </c>
@@ -1439,7 +1466,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C34" t="s">
         <v>22</v>
       </c>
@@ -1447,12 +1474,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C36" t="s">
         <v>37</v>
       </c>
@@ -1460,14 +1487,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C37" t="s">
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2975,7 +2999,7 @@
   <dimension ref="B2:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3028,7 +3052,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.45">
@@ -3103,7 +3130,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>26</v>
       </c>
@@ -3111,28 +3138,34 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
         <v>11</v>
       </c>
@@ -3140,7 +3173,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>12</v>
       </c>
@@ -3148,7 +3181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
         <v>13</v>
       </c>
@@ -3156,7 +3189,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
         <v>14</v>
       </c>
@@ -3164,12 +3197,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
         <v>27</v>
       </c>
@@ -3177,7 +3210,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
         <v>28</v>
       </c>
@@ -3185,12 +3218,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C29" t="s">
         <v>17</v>
       </c>
@@ -3198,7 +3231,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
         <v>18</v>
       </c>
@@ -3206,12 +3239,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C32" t="s">
         <v>20</v>
       </c>
@@ -3219,7 +3252,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C33" t="s">
         <v>21</v>
       </c>
@@ -3227,7 +3260,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C34" t="s">
         <v>22</v>
       </c>
@@ -3235,12 +3268,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C36" t="s">
         <v>37</v>
       </c>
@@ -3248,14 +3281,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C37" t="s">
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3273,7 +3303,7 @@
   <dimension ref="B2:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3571,7 +3601,7 @@
   <dimension ref="B2:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4166,8 +4196,8 @@
   </sheetPr>
   <dimension ref="B2:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>

</xml_diff>